<commit_message>
made changes ilisterner and excel
</commit_message>
<xml_diff>
--- a/org.dsalgo/src/test/resources/testData (1).xlsx
+++ b/org.dsalgo/src/test/resources/testData (1).xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -41,13 +42,106 @@
   </si>
   <si>
     <t>EmptyInput</t>
+  </si>
+  <si>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>confirmPassword</t>
+  </si>
+  <si>
+    <t>expectedResult</t>
+  </si>
+  <si>
+    <t>TC_01-For invalid username</t>
+  </si>
+  <si>
+    <t>john will</t>
+  </si>
+  <si>
+    <t>Starts@123</t>
+  </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
+  </si>
+  <si>
+    <t>TC_02-For invalid username</t>
+  </si>
+  <si>
+    <t>john%will</t>
+  </si>
+  <si>
+    <t>TC_03-For invalid username</t>
+  </si>
+  <si>
+    <t>john$#will</t>
+  </si>
+  <si>
+    <t>TC_04-For invalid username</t>
+  </si>
+  <si>
+    <t>aVeryVeryLongUsernameThatExceedsTheLimitOf150Characters_abcdefghijklmnopqrstuvwxyz_abcdefghijklmnopqrstuvwxyz_abcdefghijklmnopqrstuvwxyz_abcdefghijklmxyz</t>
+  </si>
+  <si>
+    <t>TC_05-For invalid password</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user1user1</t>
+  </si>
+  <si>
+    <t>TC_06-For invalid password</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>TC_07-For invalid password</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>TC_08-For password and confirm password mismatch</t>
+  </si>
+  <si>
+    <t>user5</t>
+  </si>
+  <si>
+    <t>Strong@1234</t>
+  </si>
+  <si>
+    <t>Strong@1235</t>
+  </si>
+  <si>
+    <t>TC_09-For already existing credentials</t>
+  </si>
+  <si>
+    <t>Curious_Crew</t>
+  </si>
+  <si>
+    <t>BestCrew</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -64,8 +158,22 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF004085"/>
+      <name val="-apple-system"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -76,6 +184,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCE5FF"/>
+        <bgColor rgb="FFCCE5FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -99,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -113,6 +227,27 @@
       <alignment vertical="top"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -124,6 +259,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -379,4 +518,194 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="36.63"/>
+    <col customWidth="1" min="2" max="2" width="27.25"/>
+    <col customWidth="1" min="5" max="5" width="52.75"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>